<commit_message>
Update `fiscalYears` sample data
</commit_message>
<xml_diff>
--- a/tests/bin/fixture_data.xlsx
+++ b/tests/bin/fixture_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ereiskind\nolcat\tests\bin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{171E196C-BB0C-4C2D-8A2E-4BC2F467DA30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{CA78BF5C-EF1E-480E-A1A7-41D73D9FC73A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" activeTab="4"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380"/>
   </bookViews>
   <sheets>
     <sheet name="initialize_fiscalYears" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="AUCT" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">AUCT!$A$1:$M$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">AUCT!$A$1:$K$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Sources!$A$1:$L$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
   <si>
     <t>Year</t>
   </si>
@@ -132,12 +132,6 @@
   </si>
   <si>
     <t>Fiscal Year</t>
-  </si>
-  <si>
-    <t>PK Check</t>
-  </si>
-  <si>
-    <t>R4 Ready for Upload</t>
   </si>
   <si>
     <t>Usage_Is_Being_Collected</t>
@@ -642,9 +636,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1000,22 +996,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:K1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3:I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="2" max="2" width="8.76953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.2265625" style="3" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -1041,6 +1041,90 @@
       </c>
       <c r="K1" s="1" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A2">
+        <v>2017</v>
+      </c>
+      <c r="B2" s="3">
+        <v>42552</v>
+      </c>
+      <c r="C2" s="3">
+        <v>42916</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A3">
+        <v>2018</v>
+      </c>
+      <c r="B3" s="3">
+        <v>42917</v>
+      </c>
+      <c r="C3" s="3">
+        <v>43281</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A4">
+        <v>2019</v>
+      </c>
+      <c r="B4" s="3">
+        <v>43282</v>
+      </c>
+      <c r="C4" s="3">
+        <v>43646</v>
+      </c>
+      <c r="K4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A5">
+        <v>2020</v>
+      </c>
+      <c r="B5" s="3">
+        <v>43647</v>
+      </c>
+      <c r="C5" s="3">
+        <v>44012</v>
+      </c>
+      <c r="K5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A6">
+        <v>2021</v>
+      </c>
+      <c r="B6" s="3">
+        <v>44013</v>
+      </c>
+      <c r="C6" s="3">
+        <v>44377</v>
+      </c>
+      <c r="K6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A7">
+        <v>2022</v>
+      </c>
+      <c r="B7" s="3">
+        <v>44378</v>
+      </c>
+      <c r="C7" s="3">
+        <v>44742</v>
+      </c>
+      <c r="K7">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1179,7 +1263,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
@@ -1235,10 +1319,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -1247,17 +1331,15 @@
     <col min="2" max="2" width="17.90625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.58984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.6328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.2265625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.54296875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.2265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
         <v>30</v>
       </c>
@@ -1291,15 +1373,9 @@
       <c r="K1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>42</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M1"/>
+  <autoFilter ref="A1:K1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update `vendors` sample data
</commit_message>
<xml_diff>
--- a/tests/bin/fixture_data.xlsx
+++ b/tests/bin/fixture_data.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ereiskind\nolcat\tests\bin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{CA78BF5C-EF1E-480E-A1A7-41D73D9FC73A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89977252-6BB6-4CC5-9C91-893602394019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="initialize_fiscalYears" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="48">
   <si>
     <t>Year</t>
   </si>
@@ -153,12 +153,33 @@
   </si>
   <si>
     <t>Notes</t>
+  </si>
+  <si>
+    <t>ProQuest</t>
+  </si>
+  <si>
+    <t>EBSCO</t>
+  </si>
+  <si>
+    <t>Gale</t>
+  </si>
+  <si>
+    <t>iG Publishing/BEP</t>
+  </si>
+  <si>
+    <t>Ebook Library</t>
+  </si>
+  <si>
+    <t>Ebrary</t>
+  </si>
+  <si>
+    <t>MyiLibrary</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -995,10 +1016,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I3" sqref="I3:I4"/>
     </sheetView>
   </sheetViews>
@@ -1134,14 +1155,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="1" max="1" width="12.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6796875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
@@ -1152,6 +1178,62 @@
       </c>
       <c r="C1" s="1" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.75">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.75">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.75">
+      <c r="A4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.75">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.75">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.75">
+      <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.75">
+      <c r="A8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -1160,7 +1242,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1192,7 +1274,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1254,13 +1336,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L1"/>
+  <autoFilter ref="A1:L1" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1289,7 +1371,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1318,7 +1400,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1375,7 +1457,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K1"/>
+  <autoFilter ref="A1:K1" xr:uid="{00000000-0009-0000-0000-000006000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update `statisticsSources` sample data
</commit_message>
<xml_diff>
--- a/tests/bin/fixture_data.xlsx
+++ b/tests/bin/fixture_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ereiskind\nolcat\tests\bin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89977252-6BB6-4CC5-9C91-893602394019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C42CB0E-CD3D-4A18-87E4-458439EBE141}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="initialize_fiscalYears" sheetId="1" r:id="rId1"/>
@@ -23,14 +23,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">AUCT!$A$1:$K$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Sources!$A$1:$L$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Sources!$A$1:$L$12</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="58">
   <si>
     <t>Year</t>
   </si>
@@ -174,6 +174,36 @@
   </si>
   <si>
     <t>MyiLibrary</t>
+  </si>
+  <si>
+    <t>EBSCOhost</t>
+  </si>
+  <si>
+    <t>Gale Cengage Learning</t>
+  </si>
+  <si>
+    <t>iG Library/Business Expert Press (BEP)</t>
+  </si>
+  <si>
+    <t>DemographicsNow</t>
+  </si>
+  <si>
+    <t>Ebook Central</t>
+  </si>
+  <si>
+    <t>Peterson's Career Prep</t>
+  </si>
+  <si>
+    <t>Peterson's Test Prep</t>
+  </si>
+  <si>
+    <t>Peterson's Prep</t>
+  </si>
+  <si>
+    <t>Pivot</t>
+  </si>
+  <si>
+    <t>UlrichsWeb</t>
   </si>
 </sst>
 </file>
@@ -1158,7 +1188,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -1275,20 +1305,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.2265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.40625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.76953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.76953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.2265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.40625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27.7265625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21.36328125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="31.31640625" bestFit="1" customWidth="1"/>
@@ -1299,22 +1329,22 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>24</v>
@@ -1335,8 +1365,129 @@
         <v>29</v>
       </c>
     </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="A4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="A5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="A6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="A7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="A8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="A9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="A10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="A11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="A12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:L1" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
+  <autoFilter ref="A1:L12" xr:uid="{00000000-0001-0000-0300-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Update `resourceSources` sample data
</commit_message>
<xml_diff>
--- a/tests/bin/fixture_data.xlsx
+++ b/tests/bin/fixture_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ereiskind\nolcat\tests\bin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C42CB0E-CD3D-4A18-87E4-458439EBE141}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F47E87-46FD-42FC-A412-A6B84F90DB25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,14 +23,26 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">AUCT!$A$1:$K$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Sources!$A$1:$L$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Sources!$A$1:$J$21</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="63">
   <si>
     <t>Year</t>
   </si>
@@ -104,15 +116,9 @@
     <t>`Stats` Vendor_ID</t>
   </si>
   <si>
-    <t>REFERENCE `Stats` Vendor_ID</t>
-  </si>
-  <si>
     <t>`Resource` Vendor_ID</t>
   </si>
   <si>
-    <t>REFERENCE `Resource` Vendor_ID</t>
-  </si>
-  <si>
     <t>Source_in_Use</t>
   </si>
   <si>
@@ -204,6 +210,27 @@
   </si>
   <si>
     <t>UlrichsWeb</t>
+  </si>
+  <si>
+    <t>ProQuest Congressional</t>
+  </si>
+  <si>
+    <t>ProQuest Databases</t>
+  </si>
+  <si>
+    <t>ProQuest History Vault</t>
+  </si>
+  <si>
+    <t>ProQuest Statistical Insight</t>
+  </si>
+  <si>
+    <t>ProQuest U.K. Parlimentary Papers</t>
+  </si>
+  <si>
+    <t>Statistical Abstract of the US</t>
+  </si>
+  <si>
+    <t>Ulrichsweb</t>
   </si>
 </sst>
 </file>
@@ -1212,7 +1239,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1220,7 +1247,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -1228,7 +1255,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -1236,7 +1263,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -1244,7 +1271,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -1252,7 +1279,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -1260,7 +1287,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -1305,10 +1332,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -1319,15 +1346,13 @@
     <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.2265625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.40625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.36328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="31.31640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.40625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.90625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.58984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.40625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.36328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.58984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -1347,27 +1372,21 @@
         <v>21</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.75">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1375,87 +1394,207 @@
       <c r="D2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
         <v>2</v>
       </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="F3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
         <v>3</v>
       </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="F4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
         <v>4</v>
       </c>
-      <c r="D5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="F5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>60</v>
+      </c>
+      <c r="G6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>6</v>
+      </c>
+      <c r="F7" t="s">
+        <v>61</v>
+      </c>
+      <c r="G7" t="b">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>11</v>
+      </c>
+      <c r="E8">
+        <v>7</v>
+      </c>
+      <c r="F8" t="s">
+        <v>62</v>
+      </c>
+      <c r="G8" t="b">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A9" t="s">
         <v>51</v>
-      </c>
-      <c r="C6">
-        <v>3</v>
-      </c>
-      <c r="D6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.75">
-      <c r="A7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.75">
-      <c r="A8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C8">
-        <v>3</v>
-      </c>
-      <c r="D8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.75">
-      <c r="A9" t="s">
-        <v>54</v>
       </c>
       <c r="C9">
         <v>3</v>
       </c>
       <c r="D9">
+        <v>7</v>
+      </c>
+      <c r="E9">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="F9" t="s">
+        <v>51</v>
+      </c>
+      <c r="G9" t="b">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>3</v>
+      </c>
+      <c r="J9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C10">
         <v>3</v>
@@ -1463,31 +1602,319 @@
       <c r="D10">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="E10">
+        <v>8</v>
+      </c>
+      <c r="F10" t="s">
+        <v>51</v>
+      </c>
+      <c r="G10" t="b">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>3</v>
+      </c>
+      <c r="J10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D11">
+        <v>8</v>
+      </c>
+      <c r="E11">
+        <v>9</v>
+      </c>
+      <c r="F11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G11" t="b">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>3</v>
+      </c>
+      <c r="J11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <v>9</v>
+      </c>
+      <c r="E12">
+        <v>9</v>
+      </c>
+      <c r="F12" t="s">
+        <v>52</v>
+      </c>
+      <c r="G12" t="b">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>3</v>
+      </c>
+      <c r="J12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.75">
-      <c r="A12" t="s">
-        <v>57</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12">
+      <c r="E13">
+        <v>10</v>
+      </c>
+      <c r="F13" t="s">
+        <v>54</v>
+      </c>
+      <c r="G13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14">
+        <v>5</v>
+      </c>
+      <c r="E14">
         <v>11</v>
       </c>
+      <c r="F14" t="s">
+        <v>49</v>
+      </c>
+      <c r="G14" t="b">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>3</v>
+      </c>
+      <c r="J14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>6</v>
+      </c>
+      <c r="E15">
+        <v>12</v>
+      </c>
+      <c r="F15" t="s">
+        <v>50</v>
+      </c>
+      <c r="G15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>6</v>
+      </c>
+      <c r="E16">
+        <v>13</v>
+      </c>
+      <c r="F16" t="s">
+        <v>43</v>
+      </c>
+      <c r="G16" t="b">
+        <v>0</v>
+      </c>
+      <c r="H16" s="3">
+        <v>43646</v>
+      </c>
+      <c r="I16">
+        <v>5</v>
+      </c>
+      <c r="J16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>6</v>
+      </c>
+      <c r="E17">
+        <v>14</v>
+      </c>
+      <c r="F17" t="s">
+        <v>44</v>
+      </c>
+      <c r="G17" t="b">
+        <v>0</v>
+      </c>
+      <c r="H17" s="3">
+        <v>43100</v>
+      </c>
+      <c r="I17">
+        <v>6</v>
+      </c>
+      <c r="J17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18">
+        <v>15</v>
+      </c>
+      <c r="F18" t="s">
+        <v>46</v>
+      </c>
+      <c r="G18" t="b">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>2</v>
+      </c>
+      <c r="J18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A19" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19">
+        <v>3</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
+      </c>
+      <c r="E19">
+        <v>16</v>
+      </c>
+      <c r="F19" t="s">
+        <v>47</v>
+      </c>
+      <c r="G19" t="b">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>3</v>
+      </c>
+      <c r="J19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20">
+        <v>4</v>
+      </c>
+      <c r="D20">
+        <v>4</v>
+      </c>
+      <c r="E20">
+        <v>17</v>
+      </c>
+      <c r="F20" t="s">
+        <v>48</v>
+      </c>
+      <c r="G20" t="b">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>4</v>
+      </c>
+      <c r="J20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A21" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>6</v>
+      </c>
+      <c r="E21">
+        <v>18</v>
+      </c>
+      <c r="F21" t="s">
+        <v>45</v>
+      </c>
+      <c r="G21" t="b">
+        <v>0</v>
+      </c>
+      <c r="H21" s="3">
+        <v>43646</v>
+      </c>
+      <c r="I21">
+        <v>7</v>
+      </c>
+      <c r="J21" t="b">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L12" xr:uid="{00000000-0001-0000-0300-000000000000}"/>
+  <autoFilter ref="A1:J21" xr:uid="{00000000-0001-0000-0300-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1574,37 +2001,37 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update `annualUsageCollectionTracking` sample data
</commit_message>
<xml_diff>
--- a/tests/bin/fixture_data.xlsx
+++ b/tests/bin/fixture_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ereiskind\nolcat\tests\bin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F47E87-46FD-42FC-A412-A6B84F90DB25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB7E3CF8-B4A9-4887-809B-0930E0894A34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="initialize_fiscalYears" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="81">
   <si>
     <t>Year</t>
   </si>
@@ -231,6 +231,60 @@
   </si>
   <si>
     <t>Ulrichsweb</t>
+  </si>
+  <si>
+    <t>Collection complete</t>
+  </si>
+  <si>
+    <t>Simulating a resource with usage requested by sending an email</t>
+  </si>
+  <si>
+    <t>Simulating a resource that becomes OA at the start of a calendar year</t>
+  </si>
+  <si>
+    <t>Collection not started</t>
+  </si>
+  <si>
+    <t>N/A: Open access</t>
+  </si>
+  <si>
+    <t>Usage not provided</t>
+  </si>
+  <si>
+    <t>Simulating a resource that starts offering usage statistics</t>
+  </si>
+  <si>
+    <t>Simulating a resource that's become COUNTER compliant</t>
+  </si>
+  <si>
+    <t>Collection in process (see notes)</t>
+  </si>
+  <si>
+    <t>When sending the email, note the date sent and who it was sent to</t>
+  </si>
+  <si>
+    <t>Resource became OA at start of calendar year 2018</t>
+  </si>
+  <si>
+    <t>No usage to report</t>
+  </si>
+  <si>
+    <t>Having the note about sending the email lets you know if you're in the response window, if you need to follow up, or if too much time has passed for a response to be expected</t>
+  </si>
+  <si>
+    <t>This is the first FY with usage statistics</t>
+  </si>
+  <si>
+    <t>Email info</t>
+  </si>
+  <si>
+    <t>Ended subscription, only Med has content now</t>
+  </si>
+  <si>
+    <t>N/A: Paid by Med</t>
+  </si>
+  <si>
+    <t>Still have access to content through Med</t>
   </si>
 </sst>
 </file>
@@ -714,11 +768,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -764,7 +819,29 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -775,6 +852,33 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FD17F4AF-8824-497A-BDD8-C90993DC7F1D}" name="Table1" displayName="Table1" ref="A1:K58" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:K58" xr:uid="{FD17F4AF-8824-497A-BDD8-C90993DC7F1D}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K58">
+    <sortCondition ref="B1:B58"/>
+  </sortState>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{20AA734D-6137-451E-9E97-8CB7662206B4}" name="AUCT_Statistics_Source"/>
+    <tableColumn id="2" xr3:uid="{979B2913-96F3-4FD8-92EA-2BF2A7B775AE}" name="AUCT_Fiscal_Year"/>
+    <tableColumn id="3" xr3:uid="{3B1252E2-53F3-4E04-AE14-626596D7B757}" name="Statistics Source" dataCellStyle="Normal">
+      <calculatedColumnFormula>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{BBB21629-2C5B-459B-A00D-094C1DD59867}" name="Fiscal Year" dataDxfId="0">
+      <calculatedColumnFormula>VLOOKUP(Table1[[#This Row],[AUCT_Fiscal_Year]],initialize_fiscalYears!A:B,2,0)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{4634454F-8739-4B74-8461-92AEC0C021B6}" name="Usage_Is_Being_Collected"/>
+    <tableColumn id="6" xr3:uid="{94E485CD-3F2E-409F-A3AD-66E2E5143C05}" name="Manual_Collection_Required"/>
+    <tableColumn id="7" xr3:uid="{F0F3D545-3CFB-4C50-A231-CE67E6099127}" name="Collection_Via_Email"/>
+    <tableColumn id="8" xr3:uid="{E94F7112-BF8A-4F41-A21D-C3984A47703B}" name="Is_COUNTER_Compliant"/>
+    <tableColumn id="9" xr3:uid="{AB0CE4A4-BE77-4BA1-AAE1-35277CEE52BC}" name="Collection_Status"/>
+    <tableColumn id="10" xr3:uid="{6BCF43AB-A5C5-40E4-A40F-C340DA53E84F}" name="Usage_File_Path"/>
+    <tableColumn id="11" xr3:uid="{ED77600E-5EFF-449A-A9DD-716056DF99AE}" name="Notes"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1076,133 +1180,132 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3:I4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="2" max="2" width="8.76953125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.2265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.76953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.2265625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
         <v>2017</v>
       </c>
-      <c r="B2" s="3">
+      <c r="C2" s="3">
         <v>42552</v>
       </c>
-      <c r="C2" s="3">
+      <c r="D2" s="3">
         <v>42916</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
         <v>2018</v>
       </c>
-      <c r="B3" s="3">
+      <c r="C3" s="3">
         <v>42917</v>
       </c>
-      <c r="C3" s="3">
+      <c r="D3" s="3">
         <v>43281</v>
-      </c>
-      <c r="K3">
-        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
         <v>2019</v>
       </c>
-      <c r="B4" s="3">
+      <c r="C4" s="3">
         <v>43282</v>
       </c>
-      <c r="C4" s="3">
+      <c r="D4" s="3">
         <v>43646</v>
-      </c>
-      <c r="K4">
-        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
         <v>2020</v>
       </c>
-      <c r="B5" s="3">
+      <c r="C5" s="3">
         <v>43647</v>
       </c>
-      <c r="C5" s="3">
+      <c r="D5" s="3">
         <v>44012</v>
-      </c>
-      <c r="K5">
-        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
         <v>2021</v>
       </c>
-      <c r="B6" s="3">
+      <c r="C6" s="3">
         <v>44013</v>
       </c>
-      <c r="C6" s="3">
+      <c r="D6" s="3">
         <v>44377</v>
-      </c>
-      <c r="K6">
-        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
         <v>2022</v>
       </c>
-      <c r="B7" s="3">
+      <c r="C7" s="3">
         <v>44378</v>
       </c>
-      <c r="C7" s="3">
+      <c r="D7" s="3">
         <v>44742</v>
-      </c>
-      <c r="K7">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1334,16 +1437,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16:G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="23.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.76953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.76953125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.2265625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.40625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.40625" bestFit="1" customWidth="1"/>
@@ -1354,16 +1457,16 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>20</v>
@@ -1385,11 +1488,11 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A2" t="s">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>39</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1411,11 +1514,11 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A3" t="s">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>39</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1437,11 +1540,11 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A4" t="s">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
         <v>39</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1463,11 +1566,11 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A5" t="s">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
         <v>39</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1489,11 +1592,11 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A6" t="s">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
         <v>39</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -1515,11 +1618,11 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A7" t="s">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
         <v>39</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -1541,46 +1644,46 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>46</v>
       </c>
       <c r="D8">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="E8">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="F8" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="G8" t="b">
         <v>1</v>
       </c>
       <c r="I8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J8" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A9" t="s">
-        <v>51</v>
-      </c>
-      <c r="C9">
+      <c r="A9">
         <v>3</v>
       </c>
+      <c r="B9" t="s">
+        <v>47</v>
+      </c>
       <c r="D9">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E9">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F9" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="G9" t="b">
         <v>1</v>
@@ -1589,50 +1692,50 @@
         <v>3</v>
       </c>
       <c r="J9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C10">
+      <c r="A10">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+      <c r="E10">
+        <v>17</v>
+      </c>
+      <c r="F10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G10" t="b">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>4</v>
+      </c>
+      <c r="J10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11">
         <v>3</v>
       </c>
-      <c r="D10">
-        <v>9</v>
-      </c>
-      <c r="E10">
-        <v>8</v>
-      </c>
-      <c r="F10" t="s">
-        <v>51</v>
-      </c>
-      <c r="G10" t="b">
-        <v>1</v>
-      </c>
-      <c r="I10">
-        <v>3</v>
-      </c>
-      <c r="J10" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A11" t="s">
-        <v>52</v>
-      </c>
-      <c r="C11">
-        <v>3</v>
-      </c>
-      <c r="D11">
-        <v>8</v>
-      </c>
       <c r="E11">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G11" t="b">
         <v>1</v>
@@ -1641,212 +1744,215 @@
         <v>3</v>
       </c>
       <c r="J11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A12" t="s">
+      <c r="A12">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>12</v>
+      </c>
+      <c r="F12" t="s">
+        <v>50</v>
+      </c>
+      <c r="G12" t="b">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A13">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>13</v>
+      </c>
+      <c r="F13" t="s">
+        <v>43</v>
+      </c>
+      <c r="G13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H13" s="3">
+        <v>43646</v>
+      </c>
+      <c r="I13">
+        <v>5</v>
+      </c>
+      <c r="J13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A14">
+        <v>6</v>
+      </c>
+      <c r="B14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>14</v>
+      </c>
+      <c r="F14" t="s">
+        <v>44</v>
+      </c>
+      <c r="G14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H14" s="3">
+        <v>43100</v>
+      </c>
+      <c r="I14">
+        <v>6</v>
+      </c>
+      <c r="J14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A15">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>18</v>
+      </c>
+      <c r="F15" t="s">
+        <v>45</v>
+      </c>
+      <c r="G15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H15" s="3">
+        <v>43646</v>
+      </c>
+      <c r="I15">
+        <v>7</v>
+      </c>
+      <c r="J15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A16">
+        <v>7</v>
+      </c>
+      <c r="B16" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16">
+        <v>3</v>
+      </c>
+      <c r="E16">
+        <v>8</v>
+      </c>
+      <c r="F16" t="s">
+        <v>51</v>
+      </c>
+      <c r="G16" t="b">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>3</v>
+      </c>
+      <c r="J16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A17">
+        <v>8</v>
+      </c>
+      <c r="B17" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="E17">
+        <v>9</v>
+      </c>
+      <c r="F17" t="s">
+        <v>52</v>
+      </c>
+      <c r="G17" t="b">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>3</v>
+      </c>
+      <c r="J17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A18">
+        <v>9</v>
+      </c>
+      <c r="B18" t="s">
         <v>53</v>
       </c>
-      <c r="C12">
+      <c r="D18">
         <v>3</v>
       </c>
-      <c r="D12">
+      <c r="E18">
+        <v>8</v>
+      </c>
+      <c r="F18" t="s">
+        <v>51</v>
+      </c>
+      <c r="G18" t="b">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>3</v>
+      </c>
+      <c r="J18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A19">
         <v>9</v>
       </c>
-      <c r="E12">
-        <v>9</v>
-      </c>
-      <c r="F12" t="s">
-        <v>52</v>
-      </c>
-      <c r="G12" t="b">
-        <v>1</v>
-      </c>
-      <c r="I12">
-        <v>3</v>
-      </c>
-      <c r="J12" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A13" t="s">
-        <v>54</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13">
-        <v>10</v>
-      </c>
-      <c r="E13">
-        <v>10</v>
-      </c>
-      <c r="F13" t="s">
-        <v>54</v>
-      </c>
-      <c r="G13" t="b">
-        <v>1</v>
-      </c>
-      <c r="I13">
-        <v>1</v>
-      </c>
-      <c r="J13" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A14" t="s">
-        <v>49</v>
-      </c>
-      <c r="C14">
-        <v>3</v>
-      </c>
-      <c r="D14">
-        <v>5</v>
-      </c>
-      <c r="E14">
-        <v>11</v>
-      </c>
-      <c r="F14" t="s">
-        <v>49</v>
-      </c>
-      <c r="G14" t="b">
-        <v>1</v>
-      </c>
-      <c r="I14">
-        <v>3</v>
-      </c>
-      <c r="J14" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A15" t="s">
-        <v>50</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15">
-        <v>6</v>
-      </c>
-      <c r="E15">
-        <v>12</v>
-      </c>
-      <c r="F15" t="s">
-        <v>50</v>
-      </c>
-      <c r="G15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I15">
-        <v>1</v>
-      </c>
-      <c r="J15" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A16" t="s">
-        <v>50</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16">
-        <v>6</v>
-      </c>
-      <c r="E16">
-        <v>13</v>
-      </c>
-      <c r="F16" t="s">
-        <v>43</v>
-      </c>
-      <c r="G16" t="b">
-        <v>0</v>
-      </c>
-      <c r="H16" s="3">
-        <v>43646</v>
-      </c>
-      <c r="I16">
-        <v>5</v>
-      </c>
-      <c r="J16" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A17" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17">
-        <v>6</v>
-      </c>
-      <c r="E17">
-        <v>14</v>
-      </c>
-      <c r="F17" t="s">
-        <v>44</v>
-      </c>
-      <c r="G17" t="b">
-        <v>0</v>
-      </c>
-      <c r="H17" s="3">
-        <v>43100</v>
-      </c>
-      <c r="I17">
-        <v>6</v>
-      </c>
-      <c r="J17" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A18" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18">
-        <v>2</v>
-      </c>
-      <c r="D18">
-        <v>2</v>
-      </c>
-      <c r="E18">
-        <v>15</v>
-      </c>
-      <c r="F18" t="s">
-        <v>46</v>
-      </c>
-      <c r="G18" t="b">
-        <v>1</v>
-      </c>
-      <c r="I18">
-        <v>2</v>
-      </c>
-      <c r="J18" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A19" t="s">
-        <v>47</v>
-      </c>
-      <c r="C19">
-        <v>3</v>
+      <c r="B19" t="s">
+        <v>53</v>
       </c>
       <c r="D19">
         <v>3</v>
       </c>
       <c r="E19">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="F19" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="G19" t="b">
         <v>1</v>
@@ -1859,58 +1965,55 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A20" t="s">
-        <v>48</v>
-      </c>
-      <c r="C20">
-        <v>4</v>
+      <c r="A20">
+        <v>10</v>
+      </c>
+      <c r="B20" t="s">
+        <v>54</v>
       </c>
       <c r="D20">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E20">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F20" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="G20" t="b">
         <v>1</v>
       </c>
       <c r="I20">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J20" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A21" t="s">
-        <v>50</v>
-      </c>
-      <c r="C21">
-        <v>1</v>
+      <c r="A21">
+        <v>11</v>
+      </c>
+      <c r="B21" t="s">
+        <v>55</v>
       </c>
       <c r="D21">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E21">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="F21" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="G21" t="b">
-        <v>0</v>
-      </c>
-      <c r="H21" s="3">
-        <v>43646</v>
+        <v>1</v>
       </c>
       <c r="I21">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="J21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1979,10 +2082,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -2034,8 +2137,1814 @@
         <v>38</v>
       </c>
     </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
+        <v>ProQuest</v>
+      </c>
+      <c r="D2">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Fiscal_Year]],initialize_fiscalYears!A:B,2,0)</f>
+        <v>2017</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
+        <v>EBSCOhost</v>
+      </c>
+      <c r="D3" s="4">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Fiscal_Year]],initialize_fiscalYears!A:B,2,0)</f>
+        <v>2017</v>
+      </c>
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
+        <v>Gale Cengage Learning</v>
+      </c>
+      <c r="D4" s="4">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Fiscal_Year]],initialize_fiscalYears!A:B,2,0)</f>
+        <v>2017</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
+        <v>iG Library/Business Expert Press (BEP)</v>
+      </c>
+      <c r="D5" s="4">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Fiscal_Year]],initialize_fiscalYears!A:B,2,0)</f>
+        <v>2017</v>
+      </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
+        <v>DemographicsNow</v>
+      </c>
+      <c r="D6" s="4">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Fiscal_Year]],initialize_fiscalYears!A:B,2,0)</f>
+        <v>2017</v>
+      </c>
+      <c r="E6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" t="b">
+        <v>0</v>
+      </c>
+      <c r="I6" t="s">
+        <v>63</v>
+      </c>
+      <c r="K6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
+        <v>Ebook Central</v>
+      </c>
+      <c r="D7" s="4">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Fiscal_Year]],initialize_fiscalYears!A:B,2,0)</f>
+        <v>2017</v>
+      </c>
+      <c r="E7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" t="b">
+        <v>1</v>
+      </c>
+      <c r="I7" t="s">
+        <v>63</v>
+      </c>
+      <c r="K7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
+        <v>Peterson's Career Prep</v>
+      </c>
+      <c r="D8" s="4">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Fiscal_Year]],initialize_fiscalYears!A:B,2,0)</f>
+        <v>2017</v>
+      </c>
+      <c r="E8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8" t="b">
+        <v>1</v>
+      </c>
+      <c r="G8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
+        <v>Peterson's Test Prep</v>
+      </c>
+      <c r="D9" s="4">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Fiscal_Year]],initialize_fiscalYears!A:B,2,0)</f>
+        <v>2017</v>
+      </c>
+      <c r="E9" t="b">
+        <v>1</v>
+      </c>
+      <c r="F9" t="b">
+        <v>1</v>
+      </c>
+      <c r="G9" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
+        <v>Pivot</v>
+      </c>
+      <c r="D10" s="4">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Fiscal_Year]],initialize_fiscalYears!A:B,2,0)</f>
+        <v>2017</v>
+      </c>
+      <c r="E10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H10" t="b">
+        <v>0</v>
+      </c>
+      <c r="I10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
+        <v>UlrichsWeb</v>
+      </c>
+      <c r="D11" s="4">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Fiscal_Year]],initialize_fiscalYears!A:B,2,0)</f>
+        <v>2017</v>
+      </c>
+      <c r="E11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F11" t="b">
+        <v>1</v>
+      </c>
+      <c r="G11" t="b">
+        <v>1</v>
+      </c>
+      <c r="H11" t="b">
+        <v>0</v>
+      </c>
+      <c r="I11" t="s">
+        <v>68</v>
+      </c>
+      <c r="K11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
+        <v>ProQuest</v>
+      </c>
+      <c r="D12">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Fiscal_Year]],initialize_fiscalYears!A:B,2,0)</f>
+        <v>2018</v>
+      </c>
+      <c r="E12" t="b">
+        <v>1</v>
+      </c>
+      <c r="F12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H12" t="b">
+        <v>1</v>
+      </c>
+      <c r="I12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
+        <v>EBSCOhost</v>
+      </c>
+      <c r="D13" s="4">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Fiscal_Year]],initialize_fiscalYears!A:B,2,0)</f>
+        <v>2018</v>
+      </c>
+      <c r="E13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A14">
+        <v>3</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
+        <v>Gale Cengage Learning</v>
+      </c>
+      <c r="D14" s="4">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Fiscal_Year]],initialize_fiscalYears!A:B,2,0)</f>
+        <v>2018</v>
+      </c>
+      <c r="E14" t="b">
+        <v>1</v>
+      </c>
+      <c r="F14" t="b">
+        <v>1</v>
+      </c>
+      <c r="G14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H14" t="b">
+        <v>1</v>
+      </c>
+      <c r="I14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A15">
+        <v>4</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
+        <v>iG Library/Business Expert Press (BEP)</v>
+      </c>
+      <c r="D15" s="4">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Fiscal_Year]],initialize_fiscalYears!A:B,2,0)</f>
+        <v>2018</v>
+      </c>
+      <c r="E15" t="b">
+        <v>1</v>
+      </c>
+      <c r="F15" t="b">
+        <v>1</v>
+      </c>
+      <c r="G15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I15" t="s">
+        <v>63</v>
+      </c>
+      <c r="K15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A16">
+        <v>5</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
+        <v>DemographicsNow</v>
+      </c>
+      <c r="D16" s="4">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Fiscal_Year]],initialize_fiscalYears!A:B,2,0)</f>
+        <v>2018</v>
+      </c>
+      <c r="E16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F16" t="b">
+        <v>1</v>
+      </c>
+      <c r="G16" t="b">
+        <v>1</v>
+      </c>
+      <c r="H16" t="b">
+        <v>0</v>
+      </c>
+      <c r="I16" t="s">
+        <v>71</v>
+      </c>
+      <c r="K16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A17">
+        <v>6</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
+        <v>Ebook Central</v>
+      </c>
+      <c r="D17" s="4">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Fiscal_Year]],initialize_fiscalYears!A:B,2,0)</f>
+        <v>2018</v>
+      </c>
+      <c r="E17" t="b">
+        <v>1</v>
+      </c>
+      <c r="F17" t="b">
+        <v>1</v>
+      </c>
+      <c r="G17" t="b">
+        <v>0</v>
+      </c>
+      <c r="H17" t="b">
+        <v>1</v>
+      </c>
+      <c r="I17" t="s">
+        <v>63</v>
+      </c>
+      <c r="K17" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A18">
+        <v>7</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
+        <v>Peterson's Career Prep</v>
+      </c>
+      <c r="D18" s="4">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Fiscal_Year]],initialize_fiscalYears!A:B,2,0)</f>
+        <v>2018</v>
+      </c>
+      <c r="E18" t="b">
+        <v>1</v>
+      </c>
+      <c r="F18" t="b">
+        <v>1</v>
+      </c>
+      <c r="G18" t="b">
+        <v>0</v>
+      </c>
+      <c r="H18" t="b">
+        <v>1</v>
+      </c>
+      <c r="I18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A19">
+        <v>8</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
+        <v>Peterson's Test Prep</v>
+      </c>
+      <c r="D19" s="4">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Fiscal_Year]],initialize_fiscalYears!A:B,2,0)</f>
+        <v>2018</v>
+      </c>
+      <c r="E19" t="b">
+        <v>1</v>
+      </c>
+      <c r="F19" t="b">
+        <v>1</v>
+      </c>
+      <c r="G19" t="b">
+        <v>0</v>
+      </c>
+      <c r="H19" t="b">
+        <v>1</v>
+      </c>
+      <c r="I19" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A20">
+        <v>10</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
+        <v>Pivot</v>
+      </c>
+      <c r="D20" s="4">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Fiscal_Year]],initialize_fiscalYears!A:B,2,0)</f>
+        <v>2018</v>
+      </c>
+      <c r="E20" t="b">
+        <v>0</v>
+      </c>
+      <c r="F20" t="b">
+        <v>0</v>
+      </c>
+      <c r="G20" t="b">
+        <v>0</v>
+      </c>
+      <c r="H20" t="b">
+        <v>0</v>
+      </c>
+      <c r="I20" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A21">
+        <v>11</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
+        <v>UlrichsWeb</v>
+      </c>
+      <c r="D21" s="4">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Fiscal_Year]],initialize_fiscalYears!A:B,2,0)</f>
+        <v>2018</v>
+      </c>
+      <c r="E21" t="b">
+        <v>1</v>
+      </c>
+      <c r="F21" t="b">
+        <v>1</v>
+      </c>
+      <c r="G21" t="b">
+        <v>1</v>
+      </c>
+      <c r="H21" t="b">
+        <v>0</v>
+      </c>
+      <c r="I21" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
+        <v>ProQuest</v>
+      </c>
+      <c r="D22">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Fiscal_Year]],initialize_fiscalYears!A:B,2,0)</f>
+        <v>2019</v>
+      </c>
+      <c r="E22" t="b">
+        <v>1</v>
+      </c>
+      <c r="F22" t="b">
+        <v>1</v>
+      </c>
+      <c r="G22" t="b">
+        <v>0</v>
+      </c>
+      <c r="H22" t="b">
+        <v>1</v>
+      </c>
+      <c r="I22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A23">
+        <v>2</v>
+      </c>
+      <c r="B23">
+        <v>3</v>
+      </c>
+      <c r="C23" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
+        <v>EBSCOhost</v>
+      </c>
+      <c r="D23" s="4">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Fiscal_Year]],initialize_fiscalYears!A:B,2,0)</f>
+        <v>2019</v>
+      </c>
+      <c r="E23" t="b">
+        <v>1</v>
+      </c>
+      <c r="F23" t="b">
+        <v>1</v>
+      </c>
+      <c r="G23" t="b">
+        <v>0</v>
+      </c>
+      <c r="H23" t="b">
+        <v>1</v>
+      </c>
+      <c r="I23" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A24">
+        <v>3</v>
+      </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
+      <c r="C24" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
+        <v>Gale Cengage Learning</v>
+      </c>
+      <c r="D24" s="4">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Fiscal_Year]],initialize_fiscalYears!A:B,2,0)</f>
+        <v>2019</v>
+      </c>
+      <c r="E24" t="b">
+        <v>1</v>
+      </c>
+      <c r="F24" t="b">
+        <v>1</v>
+      </c>
+      <c r="G24" t="b">
+        <v>0</v>
+      </c>
+      <c r="H24" t="b">
+        <v>1</v>
+      </c>
+      <c r="I24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A25">
+        <v>4</v>
+      </c>
+      <c r="B25">
+        <v>3</v>
+      </c>
+      <c r="C25" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
+        <v>iG Library/Business Expert Press (BEP)</v>
+      </c>
+      <c r="D25" s="4">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Fiscal_Year]],initialize_fiscalYears!A:B,2,0)</f>
+        <v>2019</v>
+      </c>
+      <c r="E25" t="b">
+        <v>1</v>
+      </c>
+      <c r="F25" t="b">
+        <v>1</v>
+      </c>
+      <c r="G25" t="b">
+        <v>0</v>
+      </c>
+      <c r="H25" t="b">
+        <v>1</v>
+      </c>
+      <c r="I25" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A26">
+        <v>5</v>
+      </c>
+      <c r="B26">
+        <v>3</v>
+      </c>
+      <c r="C26" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
+        <v>DemographicsNow</v>
+      </c>
+      <c r="D26" s="4">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Fiscal_Year]],initialize_fiscalYears!A:B,2,0)</f>
+        <v>2019</v>
+      </c>
+      <c r="E26" t="b">
+        <v>1</v>
+      </c>
+      <c r="F26" t="b">
+        <v>1</v>
+      </c>
+      <c r="G26" t="b">
+        <v>1</v>
+      </c>
+      <c r="H26" t="b">
+        <v>0</v>
+      </c>
+      <c r="I26" t="s">
+        <v>71</v>
+      </c>
+      <c r="K26" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A27">
+        <v>6</v>
+      </c>
+      <c r="B27">
+        <v>3</v>
+      </c>
+      <c r="C27" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
+        <v>Ebook Central</v>
+      </c>
+      <c r="D27" s="4">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Fiscal_Year]],initialize_fiscalYears!A:B,2,0)</f>
+        <v>2019</v>
+      </c>
+      <c r="E27" t="b">
+        <v>0</v>
+      </c>
+      <c r="F27" t="b">
+        <v>0</v>
+      </c>
+      <c r="G27" t="b">
+        <v>0</v>
+      </c>
+      <c r="H27" t="b">
+        <v>0</v>
+      </c>
+      <c r="I27" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A28">
+        <v>7</v>
+      </c>
+      <c r="B28">
+        <v>3</v>
+      </c>
+      <c r="C28" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
+        <v>Peterson's Career Prep</v>
+      </c>
+      <c r="D28" s="4">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Fiscal_Year]],initialize_fiscalYears!A:B,2,0)</f>
+        <v>2019</v>
+      </c>
+      <c r="E28" t="b">
+        <v>1</v>
+      </c>
+      <c r="F28" t="b">
+        <v>1</v>
+      </c>
+      <c r="G28" t="b">
+        <v>1</v>
+      </c>
+      <c r="H28" t="b">
+        <v>0</v>
+      </c>
+      <c r="I28" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A29">
+        <v>8</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
+        <v>Peterson's Test Prep</v>
+      </c>
+      <c r="D29" s="4">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Fiscal_Year]],initialize_fiscalYears!A:B,2,0)</f>
+        <v>2019</v>
+      </c>
+      <c r="E29" t="b">
+        <v>1</v>
+      </c>
+      <c r="F29" t="b">
+        <v>1</v>
+      </c>
+      <c r="G29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H29" t="b">
+        <v>0</v>
+      </c>
+      <c r="I29" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A30">
+        <v>10</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="C30" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
+        <v>Pivot</v>
+      </c>
+      <c r="D30" s="4">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Fiscal_Year]],initialize_fiscalYears!A:B,2,0)</f>
+        <v>2019</v>
+      </c>
+      <c r="E30" t="b">
+        <v>0</v>
+      </c>
+      <c r="F30" t="b">
+        <v>0</v>
+      </c>
+      <c r="G30" t="b">
+        <v>0</v>
+      </c>
+      <c r="H30" t="b">
+        <v>0</v>
+      </c>
+      <c r="I30" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A31">
+        <v>11</v>
+      </c>
+      <c r="B31">
+        <v>3</v>
+      </c>
+      <c r="C31" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
+        <v>UlrichsWeb</v>
+      </c>
+      <c r="D31" s="4">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Fiscal_Year]],initialize_fiscalYears!A:B,2,0)</f>
+        <v>2019</v>
+      </c>
+      <c r="E31" t="b">
+        <v>1</v>
+      </c>
+      <c r="F31" t="b">
+        <v>1</v>
+      </c>
+      <c r="G31" t="b">
+        <v>0</v>
+      </c>
+      <c r="H31" t="b">
+        <v>0</v>
+      </c>
+      <c r="I31" t="s">
+        <v>63</v>
+      </c>
+      <c r="K31" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32">
+        <v>4</v>
+      </c>
+      <c r="C32" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
+        <v>ProQuest</v>
+      </c>
+      <c r="D32">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Fiscal_Year]],initialize_fiscalYears!A:B,2,0)</f>
+        <v>2020</v>
+      </c>
+      <c r="E32" t="b">
+        <v>1</v>
+      </c>
+      <c r="F32" t="b">
+        <v>1</v>
+      </c>
+      <c r="G32" t="b">
+        <v>0</v>
+      </c>
+      <c r="H32" t="b">
+        <v>1</v>
+      </c>
+      <c r="I32" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A33">
+        <v>2</v>
+      </c>
+      <c r="B33">
+        <v>4</v>
+      </c>
+      <c r="C33" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
+        <v>EBSCOhost</v>
+      </c>
+      <c r="D33" s="4">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Fiscal_Year]],initialize_fiscalYears!A:B,2,0)</f>
+        <v>2020</v>
+      </c>
+      <c r="E33" t="b">
+        <v>1</v>
+      </c>
+      <c r="F33" t="b">
+        <v>1</v>
+      </c>
+      <c r="G33" t="b">
+        <v>0</v>
+      </c>
+      <c r="H33" t="b">
+        <v>1</v>
+      </c>
+      <c r="I33" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A34">
+        <v>3</v>
+      </c>
+      <c r="B34">
+        <v>4</v>
+      </c>
+      <c r="C34" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
+        <v>Gale Cengage Learning</v>
+      </c>
+      <c r="D34" s="4">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Fiscal_Year]],initialize_fiscalYears!A:B,2,0)</f>
+        <v>2020</v>
+      </c>
+      <c r="E34" t="b">
+        <v>1</v>
+      </c>
+      <c r="F34" t="b">
+        <v>1</v>
+      </c>
+      <c r="G34" t="b">
+        <v>0</v>
+      </c>
+      <c r="H34" t="b">
+        <v>1</v>
+      </c>
+      <c r="I34" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A35">
+        <v>4</v>
+      </c>
+      <c r="B35">
+        <v>4</v>
+      </c>
+      <c r="C35" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
+        <v>iG Library/Business Expert Press (BEP)</v>
+      </c>
+      <c r="D35" s="4">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Fiscal_Year]],initialize_fiscalYears!A:B,2,0)</f>
+        <v>2020</v>
+      </c>
+      <c r="E35" t="b">
+        <v>1</v>
+      </c>
+      <c r="F35" t="b">
+        <v>1</v>
+      </c>
+      <c r="G35" t="b">
+        <v>0</v>
+      </c>
+      <c r="H35" t="b">
+        <v>1</v>
+      </c>
+      <c r="I35" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A36">
+        <v>5</v>
+      </c>
+      <c r="B36">
+        <v>4</v>
+      </c>
+      <c r="C36" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
+        <v>DemographicsNow</v>
+      </c>
+      <c r="D36" s="4">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Fiscal_Year]],initialize_fiscalYears!A:B,2,0)</f>
+        <v>2020</v>
+      </c>
+      <c r="E36" t="b">
+        <v>1</v>
+      </c>
+      <c r="F36" t="b">
+        <v>1</v>
+      </c>
+      <c r="G36" t="b">
+        <v>1</v>
+      </c>
+      <c r="H36" t="b">
+        <v>0</v>
+      </c>
+      <c r="I36" t="s">
+        <v>71</v>
+      </c>
+      <c r="K36" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A37">
+        <v>6</v>
+      </c>
+      <c r="B37">
+        <v>4</v>
+      </c>
+      <c r="C37" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
+        <v>Ebook Central</v>
+      </c>
+      <c r="D37" s="4">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Fiscal_Year]],initialize_fiscalYears!A:B,2,0)</f>
+        <v>2020</v>
+      </c>
+      <c r="E37" t="b">
+        <v>0</v>
+      </c>
+      <c r="F37" t="b">
+        <v>0</v>
+      </c>
+      <c r="G37" t="b">
+        <v>0</v>
+      </c>
+      <c r="H37" t="b">
+        <v>0</v>
+      </c>
+      <c r="I37" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A38">
+        <v>9</v>
+      </c>
+      <c r="B38">
+        <v>4</v>
+      </c>
+      <c r="C38" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
+        <v>Peterson's Prep</v>
+      </c>
+      <c r="D38" s="4">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Fiscal_Year]],initialize_fiscalYears!A:B,2,0)</f>
+        <v>2020</v>
+      </c>
+      <c r="E38" t="b">
+        <v>1</v>
+      </c>
+      <c r="F38" t="b">
+        <v>1</v>
+      </c>
+      <c r="G38" t="b">
+        <v>0</v>
+      </c>
+      <c r="H38" t="b">
+        <v>0</v>
+      </c>
+      <c r="I38" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A39">
+        <v>10</v>
+      </c>
+      <c r="B39">
+        <v>4</v>
+      </c>
+      <c r="C39" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
+        <v>Pivot</v>
+      </c>
+      <c r="D39" s="4">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Fiscal_Year]],initialize_fiscalYears!A:B,2,0)</f>
+        <v>2020</v>
+      </c>
+      <c r="E39" t="b">
+        <v>0</v>
+      </c>
+      <c r="F39" t="b">
+        <v>0</v>
+      </c>
+      <c r="G39" t="b">
+        <v>0</v>
+      </c>
+      <c r="H39" t="b">
+        <v>0</v>
+      </c>
+      <c r="I39" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A40">
+        <v>11</v>
+      </c>
+      <c r="B40">
+        <v>4</v>
+      </c>
+      <c r="C40" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
+        <v>UlrichsWeb</v>
+      </c>
+      <c r="D40" s="4">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Fiscal_Year]],initialize_fiscalYears!A:B,2,0)</f>
+        <v>2020</v>
+      </c>
+      <c r="E40" t="b">
+        <v>1</v>
+      </c>
+      <c r="F40" t="b">
+        <v>1</v>
+      </c>
+      <c r="G40" t="b">
+        <v>0</v>
+      </c>
+      <c r="H40" t="b">
+        <v>0</v>
+      </c>
+      <c r="I40" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A41">
+        <v>1</v>
+      </c>
+      <c r="B41">
+        <v>5</v>
+      </c>
+      <c r="C41" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
+        <v>ProQuest</v>
+      </c>
+      <c r="D41">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Fiscal_Year]],initialize_fiscalYears!A:B,2,0)</f>
+        <v>2021</v>
+      </c>
+      <c r="E41" t="b">
+        <v>1</v>
+      </c>
+      <c r="F41" t="b">
+        <v>1</v>
+      </c>
+      <c r="G41" t="b">
+        <v>0</v>
+      </c>
+      <c r="H41" t="b">
+        <v>1</v>
+      </c>
+      <c r="I41" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A42">
+        <v>2</v>
+      </c>
+      <c r="B42">
+        <v>5</v>
+      </c>
+      <c r="C42" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
+        <v>EBSCOhost</v>
+      </c>
+      <c r="D42" s="4">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Fiscal_Year]],initialize_fiscalYears!A:B,2,0)</f>
+        <v>2021</v>
+      </c>
+      <c r="E42" t="b">
+        <v>1</v>
+      </c>
+      <c r="F42" t="b">
+        <v>1</v>
+      </c>
+      <c r="G42" t="b">
+        <v>0</v>
+      </c>
+      <c r="H42" t="b">
+        <v>1</v>
+      </c>
+      <c r="I42" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A43">
+        <v>3</v>
+      </c>
+      <c r="B43">
+        <v>5</v>
+      </c>
+      <c r="C43" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
+        <v>Gale Cengage Learning</v>
+      </c>
+      <c r="D43" s="4">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Fiscal_Year]],initialize_fiscalYears!A:B,2,0)</f>
+        <v>2021</v>
+      </c>
+      <c r="E43" t="b">
+        <v>1</v>
+      </c>
+      <c r="F43" t="b">
+        <v>1</v>
+      </c>
+      <c r="G43" t="b">
+        <v>0</v>
+      </c>
+      <c r="H43" t="b">
+        <v>1</v>
+      </c>
+      <c r="I43" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A44">
+        <v>4</v>
+      </c>
+      <c r="B44">
+        <v>5</v>
+      </c>
+      <c r="C44" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
+        <v>iG Library/Business Expert Press (BEP)</v>
+      </c>
+      <c r="D44" s="4">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Fiscal_Year]],initialize_fiscalYears!A:B,2,0)</f>
+        <v>2021</v>
+      </c>
+      <c r="E44" t="b">
+        <v>1</v>
+      </c>
+      <c r="F44" t="b">
+        <v>1</v>
+      </c>
+      <c r="G44" t="b">
+        <v>0</v>
+      </c>
+      <c r="H44" t="b">
+        <v>1</v>
+      </c>
+      <c r="I44" t="s">
+        <v>63</v>
+      </c>
+      <c r="K44" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A45">
+        <v>5</v>
+      </c>
+      <c r="B45">
+        <v>5</v>
+      </c>
+      <c r="C45" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
+        <v>DemographicsNow</v>
+      </c>
+      <c r="D45" s="4">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Fiscal_Year]],initialize_fiscalYears!A:B,2,0)</f>
+        <v>2021</v>
+      </c>
+      <c r="E45" t="b">
+        <v>1</v>
+      </c>
+      <c r="F45" t="b">
+        <v>1</v>
+      </c>
+      <c r="G45" t="b">
+        <v>1</v>
+      </c>
+      <c r="H45" t="b">
+        <v>0</v>
+      </c>
+      <c r="I45" t="s">
+        <v>71</v>
+      </c>
+      <c r="K45" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A46">
+        <v>6</v>
+      </c>
+      <c r="B46">
+        <v>5</v>
+      </c>
+      <c r="C46" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
+        <v>Ebook Central</v>
+      </c>
+      <c r="D46" s="4">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Fiscal_Year]],initialize_fiscalYears!A:B,2,0)</f>
+        <v>2021</v>
+      </c>
+      <c r="E46" t="b">
+        <v>0</v>
+      </c>
+      <c r="F46" t="b">
+        <v>0</v>
+      </c>
+      <c r="G46" t="b">
+        <v>0</v>
+      </c>
+      <c r="H46" t="b">
+        <v>0</v>
+      </c>
+      <c r="I46" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A47">
+        <v>9</v>
+      </c>
+      <c r="B47">
+        <v>5</v>
+      </c>
+      <c r="C47" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
+        <v>Peterson's Prep</v>
+      </c>
+      <c r="D47" s="4">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Fiscal_Year]],initialize_fiscalYears!A:B,2,0)</f>
+        <v>2021</v>
+      </c>
+      <c r="E47" t="b">
+        <v>1</v>
+      </c>
+      <c r="F47" t="b">
+        <v>1</v>
+      </c>
+      <c r="G47" t="b">
+        <v>0</v>
+      </c>
+      <c r="H47" t="b">
+        <v>0</v>
+      </c>
+      <c r="I47" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A48">
+        <v>10</v>
+      </c>
+      <c r="B48">
+        <v>5</v>
+      </c>
+      <c r="C48" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
+        <v>Pivot</v>
+      </c>
+      <c r="D48" s="4">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Fiscal_Year]],initialize_fiscalYears!A:B,2,0)</f>
+        <v>2021</v>
+      </c>
+      <c r="E48" t="b">
+        <v>0</v>
+      </c>
+      <c r="F48" t="b">
+        <v>0</v>
+      </c>
+      <c r="G48" t="b">
+        <v>0</v>
+      </c>
+      <c r="H48" t="b">
+        <v>0</v>
+      </c>
+      <c r="I48" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A49">
+        <v>11</v>
+      </c>
+      <c r="B49">
+        <v>5</v>
+      </c>
+      <c r="C49" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
+        <v>UlrichsWeb</v>
+      </c>
+      <c r="D49" s="4">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Fiscal_Year]],initialize_fiscalYears!A:B,2,0)</f>
+        <v>2021</v>
+      </c>
+      <c r="E49" t="b">
+        <v>1</v>
+      </c>
+      <c r="F49" t="b">
+        <v>1</v>
+      </c>
+      <c r="G49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I49" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A50">
+        <v>1</v>
+      </c>
+      <c r="B50">
+        <v>6</v>
+      </c>
+      <c r="C50" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
+        <v>ProQuest</v>
+      </c>
+      <c r="D50">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Fiscal_Year]],initialize_fiscalYears!A:B,2,0)</f>
+        <v>2022</v>
+      </c>
+      <c r="E50" t="b">
+        <v>1</v>
+      </c>
+      <c r="F50" t="b">
+        <v>1</v>
+      </c>
+      <c r="G50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H50" t="b">
+        <v>1</v>
+      </c>
+      <c r="I50" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A51">
+        <v>2</v>
+      </c>
+      <c r="B51">
+        <v>6</v>
+      </c>
+      <c r="C51" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
+        <v>EBSCOhost</v>
+      </c>
+      <c r="D51" s="4">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Fiscal_Year]],initialize_fiscalYears!A:B,2,0)</f>
+        <v>2022</v>
+      </c>
+      <c r="E51" t="b">
+        <v>1</v>
+      </c>
+      <c r="F51" t="b">
+        <v>1</v>
+      </c>
+      <c r="G51" t="b">
+        <v>0</v>
+      </c>
+      <c r="H51" t="b">
+        <v>1</v>
+      </c>
+      <c r="I51" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A52">
+        <v>3</v>
+      </c>
+      <c r="B52">
+        <v>6</v>
+      </c>
+      <c r="C52" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
+        <v>Gale Cengage Learning</v>
+      </c>
+      <c r="D52" s="4">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Fiscal_Year]],initialize_fiscalYears!A:B,2,0)</f>
+        <v>2022</v>
+      </c>
+      <c r="E52" t="b">
+        <v>1</v>
+      </c>
+      <c r="F52" t="b">
+        <v>1</v>
+      </c>
+      <c r="G52" t="b">
+        <v>0</v>
+      </c>
+      <c r="H52" t="b">
+        <v>1</v>
+      </c>
+      <c r="I52" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A53">
+        <v>4</v>
+      </c>
+      <c r="B53">
+        <v>6</v>
+      </c>
+      <c r="C53" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
+        <v>iG Library/Business Expert Press (BEP)</v>
+      </c>
+      <c r="D53" s="4">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Fiscal_Year]],initialize_fiscalYears!A:B,2,0)</f>
+        <v>2022</v>
+      </c>
+      <c r="E53" t="b">
+        <v>0</v>
+      </c>
+      <c r="F53" t="b">
+        <v>0</v>
+      </c>
+      <c r="G53" t="b">
+        <v>0</v>
+      </c>
+      <c r="H53" t="b">
+        <v>0</v>
+      </c>
+      <c r="I53" t="s">
+        <v>79</v>
+      </c>
+      <c r="K53" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A54">
+        <v>5</v>
+      </c>
+      <c r="B54">
+        <v>6</v>
+      </c>
+      <c r="C54" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
+        <v>DemographicsNow</v>
+      </c>
+      <c r="D54" s="4">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Fiscal_Year]],initialize_fiscalYears!A:B,2,0)</f>
+        <v>2022</v>
+      </c>
+      <c r="E54" t="b">
+        <v>1</v>
+      </c>
+      <c r="F54" t="b">
+        <v>1</v>
+      </c>
+      <c r="G54" t="b">
+        <v>1</v>
+      </c>
+      <c r="H54" t="b">
+        <v>0</v>
+      </c>
+      <c r="I54" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A55">
+        <v>6</v>
+      </c>
+      <c r="B55">
+        <v>6</v>
+      </c>
+      <c r="C55" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
+        <v>Ebook Central</v>
+      </c>
+      <c r="D55" s="4">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Fiscal_Year]],initialize_fiscalYears!A:B,2,0)</f>
+        <v>2022</v>
+      </c>
+      <c r="E55" t="b">
+        <v>0</v>
+      </c>
+      <c r="F55" t="b">
+        <v>0</v>
+      </c>
+      <c r="G55" t="b">
+        <v>0</v>
+      </c>
+      <c r="H55" t="b">
+        <v>0</v>
+      </c>
+      <c r="I55" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A56">
+        <v>9</v>
+      </c>
+      <c r="B56">
+        <v>6</v>
+      </c>
+      <c r="C56" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
+        <v>Peterson's Prep</v>
+      </c>
+      <c r="D56" s="4">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Fiscal_Year]],initialize_fiscalYears!A:B,2,0)</f>
+        <v>2022</v>
+      </c>
+      <c r="E56" t="b">
+        <v>1</v>
+      </c>
+      <c r="F56" t="b">
+        <v>1</v>
+      </c>
+      <c r="G56" t="b">
+        <v>0</v>
+      </c>
+      <c r="H56" t="b">
+        <v>0</v>
+      </c>
+      <c r="I56" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A57">
+        <v>10</v>
+      </c>
+      <c r="B57">
+        <v>6</v>
+      </c>
+      <c r="C57" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
+        <v>Pivot</v>
+      </c>
+      <c r="D57" s="4">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Fiscal_Year]],initialize_fiscalYears!A:B,2,0)</f>
+        <v>2022</v>
+      </c>
+      <c r="E57" t="b">
+        <v>0</v>
+      </c>
+      <c r="F57" t="b">
+        <v>0</v>
+      </c>
+      <c r="G57" t="b">
+        <v>0</v>
+      </c>
+      <c r="H57" t="b">
+        <v>0</v>
+      </c>
+      <c r="I57" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A58">
+        <v>11</v>
+      </c>
+      <c r="B58">
+        <v>6</v>
+      </c>
+      <c r="C58" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
+        <v>UlrichsWeb</v>
+      </c>
+      <c r="D58" s="4">
+        <f>VLOOKUP(Table1[[#This Row],[AUCT_Fiscal_Year]],initialize_fiscalYears!A:B,2,0)</f>
+        <v>2022</v>
+      </c>
+      <c r="E58" t="b">
+        <v>1</v>
+      </c>
+      <c r="F58" t="b">
+        <v>1</v>
+      </c>
+      <c r="G58" t="b">
+        <v>0</v>
+      </c>
+      <c r="H58" t="b">
+        <v>0</v>
+      </c>
+      <c r="I58" t="s">
+        <v>66</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:K1" xr:uid="{00000000-0009-0000-0000-000006000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Make all fixtures zero-indexed
</commit_message>
<xml_diff>
--- a/tests/bin/fixture_data.xlsx
+++ b/tests/bin/fixture_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ereiskind\nolcat\tests\bin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E06E1B96-7035-498E-9143-FF644EEC6A06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82A0379E-5CCB-413E-AD73-FE33013E575B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" firstSheet="6" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="initialize_fiscalYears" sheetId="1" r:id="rId1"/>
@@ -1726,15 +1726,15 @@
       </font>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFFFFF00"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1926,7 +1926,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A4A8541E-35DC-4119-8777-B6D1B630514B}" name="Table26" displayName="Table26" ref="A1:H88" totalsRowShown="0">
   <autoFilter ref="A1:H88" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H88">
-    <sortCondition sortBy="cellColor" ref="A1:A88" dxfId="10"/>
+    <sortCondition sortBy="cellColor" ref="A1:A88" dxfId="11"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="resource_platform_ID"/>
@@ -1953,7 +1953,7 @@
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Metric_Type"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Data_Type"/>
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Section_Type"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Usage_Date" dataDxfId="11"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Usage_Date" dataDxfId="10"/>
     <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Usage_Count"/>
     <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="resource_platform_ID"/>
   </tableColumns>
@@ -2260,7 +2260,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
@@ -2306,7 +2308,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>2017</v>
@@ -2320,7 +2322,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>2018</v>
@@ -2334,7 +2336,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>2019</v>
@@ -2348,7 +2350,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>2020</v>
@@ -2362,7 +2364,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>2021</v>
@@ -2376,7 +2378,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>2022</v>
@@ -38352,8 +38354,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -38379,7 +38381,7 @@
         <v>39</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.75">
@@ -38387,7 +38389,7 @@
         <v>40</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.75">
@@ -38395,7 +38397,7 @@
         <v>41</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.75">
@@ -38403,7 +38405,7 @@
         <v>42</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.75">
@@ -38411,7 +38413,7 @@
         <v>43</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.75">
@@ -38419,7 +38421,7 @@
         <v>44</v>
       </c>
       <c r="C7">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.75">
@@ -38427,7 +38429,7 @@
         <v>45</v>
       </c>
       <c r="C8">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -38471,8 +38473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:G17"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -38523,16 +38525,16 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>39</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" t="s">
         <v>56</v>
@@ -38541,7 +38543,7 @@
         <v>1</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2" t="b">
         <v>1</v>
@@ -38549,16 +38551,16 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
         <v>39</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3" t="s">
         <v>57</v>
@@ -38567,7 +38569,7 @@
         <v>1</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3" t="b">
         <v>1</v>
@@ -38575,16 +38577,16 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4" t="s">
         <v>39</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F4" t="s">
         <v>58</v>
@@ -38593,7 +38595,7 @@
         <v>1</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4" t="b">
         <v>1</v>
@@ -38601,16 +38603,16 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B5" t="s">
         <v>39</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F5" t="s">
         <v>59</v>
@@ -38619,7 +38621,7 @@
         <v>1</v>
       </c>
       <c r="I5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J5" t="b">
         <v>1</v>
@@ -38627,16 +38629,16 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B6" t="s">
         <v>39</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F6" t="s">
         <v>60</v>
@@ -38645,7 +38647,7 @@
         <v>1</v>
       </c>
       <c r="I6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J6" t="b">
         <v>1</v>
@@ -38653,16 +38655,16 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B7" t="s">
         <v>39</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F7" t="s">
         <v>61</v>
@@ -38671,7 +38673,7 @@
         <v>1</v>
       </c>
       <c r="I7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7" t="b">
         <v>1</v>
@@ -38679,16 +38681,16 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B8" t="s">
         <v>46</v>
       </c>
       <c r="D8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E8">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F8" t="s">
         <v>46</v>
@@ -38697,7 +38699,7 @@
         <v>1</v>
       </c>
       <c r="I8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J8" t="b">
         <v>1</v>
@@ -38705,16 +38707,16 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B9" t="s">
         <v>47</v>
       </c>
       <c r="D9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E9">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F9" t="s">
         <v>47</v>
@@ -38723,7 +38725,7 @@
         <v>1</v>
       </c>
       <c r="I9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J9" t="b">
         <v>1</v>
@@ -38731,16 +38733,16 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B10" t="s">
         <v>48</v>
       </c>
       <c r="D10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E10">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F10" t="s">
         <v>48</v>
@@ -38749,7 +38751,7 @@
         <v>1</v>
       </c>
       <c r="I10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J10" t="b">
         <v>1</v>
@@ -38757,16 +38759,16 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A11">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B11" t="s">
         <v>49</v>
       </c>
       <c r="D11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E11">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F11" t="s">
         <v>49</v>
@@ -38775,7 +38777,7 @@
         <v>1</v>
       </c>
       <c r="I11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J11" t="b">
         <v>1</v>
@@ -38783,16 +38785,16 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A12">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B12" t="s">
         <v>50</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F12" t="s">
         <v>50</v>
@@ -38801,7 +38803,7 @@
         <v>1</v>
       </c>
       <c r="I12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12" t="b">
         <v>1</v>
@@ -38809,16 +38811,16 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A13">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B13" t="s">
         <v>50</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F13" t="s">
         <v>43</v>
@@ -38830,7 +38832,7 @@
         <v>43646</v>
       </c>
       <c r="I13">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J13" t="b">
         <v>0</v>
@@ -38838,16 +38840,16 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A14">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B14" t="s">
         <v>50</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F14" t="s">
         <v>44</v>
@@ -38859,7 +38861,7 @@
         <v>43100</v>
       </c>
       <c r="I14">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J14" t="b">
         <v>0</v>
@@ -38867,16 +38869,16 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A15">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B15" t="s">
         <v>50</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F15" t="s">
         <v>45</v>
@@ -38888,7 +38890,7 @@
         <v>43646</v>
       </c>
       <c r="I15">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J15" t="b">
         <v>0</v>
@@ -38896,16 +38898,16 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A16">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B16" t="s">
         <v>51</v>
       </c>
       <c r="D16">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E16">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F16" t="s">
         <v>51</v>
@@ -38914,7 +38916,7 @@
         <v>1</v>
       </c>
       <c r="I16">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J16" t="b">
         <v>0</v>
@@ -38922,16 +38924,16 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A17">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B17" t="s">
         <v>52</v>
       </c>
       <c r="D17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E17">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F17" t="s">
         <v>52</v>
@@ -38940,7 +38942,7 @@
         <v>1</v>
       </c>
       <c r="I17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J17" t="b">
         <v>0</v>
@@ -38948,16 +38950,16 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A18">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B18" t="s">
         <v>53</v>
       </c>
       <c r="D18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E18">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F18" t="s">
         <v>51</v>
@@ -38966,7 +38968,7 @@
         <v>1</v>
       </c>
       <c r="I18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J18" t="b">
         <v>1</v>
@@ -38974,16 +38976,16 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A19">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B19" t="s">
         <v>53</v>
       </c>
       <c r="D19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E19">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F19" t="s">
         <v>52</v>
@@ -38992,7 +38994,7 @@
         <v>1</v>
       </c>
       <c r="I19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J19" t="b">
         <v>1</v>
@@ -39000,16 +39002,16 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A20">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B20" t="s">
         <v>54</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E20">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F20" t="s">
         <v>54</v>
@@ -39018,7 +39020,7 @@
         <v>1</v>
       </c>
       <c r="I20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J20" t="b">
         <v>1</v>
@@ -39026,16 +39028,16 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A21">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B21" t="s">
         <v>55</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F21" t="s">
         <v>62</v>
@@ -39044,7 +39046,7 @@
         <v>1</v>
       </c>
       <c r="I21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J21" t="b">
         <v>1</v>
@@ -39119,7 +39121,7 @@
   <dimension ref="A1:K58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -39173,10 +39175,10 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
@@ -39204,10 +39206,10 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
@@ -39235,10 +39237,10 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
@@ -39266,10 +39268,10 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
@@ -39297,10 +39299,10 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
@@ -39331,10 +39333,10 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
@@ -39365,10 +39367,10 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
@@ -39396,10 +39398,10 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
@@ -39427,10 +39429,10 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A10">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
@@ -39458,10 +39460,10 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A11">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
@@ -39492,10 +39494,10 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C12" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
@@ -39523,10 +39525,10 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C13" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
@@ -39554,10 +39556,10 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C14" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
@@ -39585,10 +39587,10 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A15">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C15" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
@@ -39619,10 +39621,10 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A16">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C16" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
@@ -39653,10 +39655,10 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A17">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C17" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
@@ -39687,10 +39689,10 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A18">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C18" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
@@ -39718,10 +39720,10 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A19">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C19" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
@@ -39749,10 +39751,10 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A20">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C20" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
@@ -39780,10 +39782,10 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A21">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C21" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
@@ -39811,10 +39813,10 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B22">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C22" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
@@ -39842,10 +39844,10 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23">
         <v>2</v>
-      </c>
-      <c r="B23">
-        <v>3</v>
       </c>
       <c r="C23" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
@@ -39873,10 +39875,10 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A24">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B24">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C24" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
@@ -39904,10 +39906,10 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A25">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B25">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C25" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
@@ -39935,10 +39937,10 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A26">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B26">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C26" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
@@ -39969,10 +39971,10 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A27">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B27">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C27" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
@@ -40000,10 +40002,10 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A28">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B28">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C28" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
@@ -40031,10 +40033,10 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A29">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B29">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C29" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
@@ -40062,10 +40064,10 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A30">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B30">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C30" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
@@ -40093,10 +40095,10 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A31">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B31">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C31" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
@@ -40127,10 +40129,10 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B32">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C32" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
@@ -40158,10 +40160,10 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A33">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B33">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C33" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
@@ -40189,10 +40191,10 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A34">
+        <v>2</v>
+      </c>
+      <c r="B34">
         <v>3</v>
-      </c>
-      <c r="B34">
-        <v>4</v>
       </c>
       <c r="C34" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
@@ -40220,10 +40222,10 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A35">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B35">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C35" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
@@ -40251,10 +40253,10 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A36">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B36">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C36" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
@@ -40285,10 +40287,10 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A37">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B37">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C37" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
@@ -40316,10 +40318,10 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A38">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B38">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C38" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
@@ -40347,10 +40349,10 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A39">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B39">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C39" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
@@ -40378,10 +40380,10 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A40">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B40">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C40" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
@@ -40409,10 +40411,10 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B41">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C41" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
@@ -40440,10 +40442,10 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A42">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B42">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C42" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
@@ -40471,10 +40473,10 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A43">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B43">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C43" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
@@ -40502,10 +40504,10 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A44">
+        <v>3</v>
+      </c>
+      <c r="B44">
         <v>4</v>
-      </c>
-      <c r="B44">
-        <v>5</v>
       </c>
       <c r="C44" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
@@ -40536,10 +40538,10 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A45">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B45">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C45" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
@@ -40570,10 +40572,10 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A46">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B46">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C46" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
@@ -40601,10 +40603,10 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A47">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B47">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C47" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
@@ -40632,10 +40634,10 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A48">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B48">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C48" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
@@ -40663,10 +40665,10 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A49">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B49">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C49" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
@@ -40694,10 +40696,10 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B50">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C50" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
@@ -40725,10 +40727,10 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A51">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B51">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C51" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
@@ -40756,10 +40758,10 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A52">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B52">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C52" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
@@ -40787,10 +40789,10 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A53">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B53">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C53" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
@@ -40821,10 +40823,10 @@
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A54">
+        <v>4</v>
+      </c>
+      <c r="B54">
         <v>5</v>
-      </c>
-      <c r="B54">
-        <v>6</v>
       </c>
       <c r="C54" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
@@ -40852,10 +40854,10 @@
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A55">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B55">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C55" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
@@ -40883,10 +40885,10 @@
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A56">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B56">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C56" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
@@ -40914,10 +40916,10 @@
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A57">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B57">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C57" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
@@ -40945,10 +40947,10 @@
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A58">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B58">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C58" t="str">
         <f>VLOOKUP(Table1[[#This Row],[AUCT_Statistics_Source]],Sources!A:B,2,0)</f>
@@ -43518,13 +43520,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E43:E47">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E60:E105">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E106:E148">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -43537,8 +43539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E03B838-864A-4456-883C-E1968C11F1AE}">
   <dimension ref="A1:H88"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -43589,7 +43591,7 @@
         <v>39</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -43606,7 +43608,7 @@
         <v>272</v>
       </c>
       <c r="G3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -43623,7 +43625,7 @@
         <v>39</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4">
         <v>2</v>
@@ -43640,7 +43642,7 @@
         <v>46</v>
       </c>
       <c r="G5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H5">
         <v>2</v>
@@ -43660,7 +43662,7 @@
         <v>352</v>
       </c>
       <c r="G6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H6">
         <v>3</v>
@@ -43677,7 +43679,7 @@
         <v>39</v>
       </c>
       <c r="G7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H7">
         <v>3</v>
@@ -43697,7 +43699,7 @@
         <v>351</v>
       </c>
       <c r="G8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H8">
         <v>3</v>
@@ -43714,7 +43716,7 @@
         <v>272</v>
       </c>
       <c r="G9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H9">
         <v>3</v>
@@ -43731,7 +43733,7 @@
         <v>39</v>
       </c>
       <c r="G10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H10">
         <v>4</v>
@@ -43748,7 +43750,7 @@
         <v>39</v>
       </c>
       <c r="G11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H11">
         <v>5</v>
@@ -43768,7 +43770,7 @@
         <v>350</v>
       </c>
       <c r="G12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H12">
         <v>5</v>
@@ -43785,7 +43787,7 @@
         <v>272</v>
       </c>
       <c r="G13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H13">
         <v>5</v>
@@ -43802,7 +43804,7 @@
         <v>46</v>
       </c>
       <c r="G14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H14">
         <v>6</v>
@@ -43819,7 +43821,7 @@
         <v>272</v>
       </c>
       <c r="G15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H15">
         <v>6</v>
@@ -43839,7 +43841,7 @@
         <v>349</v>
       </c>
       <c r="G16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H16">
         <v>7</v>
@@ -43856,7 +43858,7 @@
         <v>39</v>
       </c>
       <c r="G17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H17">
         <v>8</v>
@@ -43876,7 +43878,7 @@
         <v>348</v>
       </c>
       <c r="G18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H18">
         <v>9</v>
@@ -43896,7 +43898,7 @@
         <v>347</v>
       </c>
       <c r="G19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H19">
         <v>10</v>
@@ -43913,7 +43915,7 @@
         <v>272</v>
       </c>
       <c r="G20">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H20">
         <v>10</v>
@@ -43933,7 +43935,7 @@
         <v>346</v>
       </c>
       <c r="G21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H21">
         <v>11</v>
@@ -43950,7 +43952,7 @@
         <v>272</v>
       </c>
       <c r="G22">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H22">
         <v>11</v>
@@ -43970,7 +43972,7 @@
         <v>345</v>
       </c>
       <c r="G23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H23">
         <v>12</v>
@@ -43990,7 +43992,7 @@
         <v>344</v>
       </c>
       <c r="G24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H24">
         <v>13</v>
@@ -44007,7 +44009,7 @@
         <v>39</v>
       </c>
       <c r="G25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H25">
         <v>13</v>
@@ -44024,7 +44026,7 @@
         <v>272</v>
       </c>
       <c r="G26">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H26">
         <v>13</v>
@@ -44041,7 +44043,7 @@
         <v>39</v>
       </c>
       <c r="G27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H27">
         <v>14</v>
@@ -44061,7 +44063,7 @@
         <v>283</v>
       </c>
       <c r="G28">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H28">
         <v>15</v>
@@ -44078,7 +44080,7 @@
         <v>39</v>
       </c>
       <c r="G29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H29">
         <v>16</v>
@@ -44095,7 +44097,7 @@
         <v>46</v>
       </c>
       <c r="G30">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H30">
         <v>17</v>
@@ -44112,7 +44114,7 @@
         <v>39</v>
       </c>
       <c r="G31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H31">
         <v>18</v>
@@ -44132,7 +44134,7 @@
         <v>343</v>
       </c>
       <c r="G32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H32">
         <v>19</v>
@@ -44152,7 +44154,7 @@
         <v>342</v>
       </c>
       <c r="G33">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H33">
         <v>20</v>
@@ -44172,7 +44174,7 @@
         <v>341</v>
       </c>
       <c r="G34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H34">
         <v>20</v>
@@ -44192,7 +44194,7 @@
         <v>340</v>
       </c>
       <c r="G35">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H35">
         <v>21</v>
@@ -44209,7 +44211,7 @@
         <v>39</v>
       </c>
       <c r="G36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H36">
         <v>22</v>
@@ -44229,7 +44231,7 @@
         <v>339</v>
       </c>
       <c r="G37">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H37">
         <v>23</v>
@@ -44243,7 +44245,7 @@
         <v>46</v>
       </c>
       <c r="G38">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H38">
         <v>24</v>
@@ -44263,7 +44265,7 @@
         <v>279</v>
       </c>
       <c r="G39">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H39">
         <v>25</v>
@@ -44283,7 +44285,7 @@
         <v>338</v>
       </c>
       <c r="G40">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H40">
         <v>26</v>
@@ -44303,7 +44305,7 @@
         <v>337</v>
       </c>
       <c r="G41">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H41">
         <v>28</v>
@@ -44323,7 +44325,7 @@
         <v>336</v>
       </c>
       <c r="G42">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H42">
         <v>29</v>
@@ -44343,7 +44345,7 @@
         <v>335</v>
       </c>
       <c r="G43">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H43">
         <v>30</v>
@@ -44363,7 +44365,7 @@
         <v>334</v>
       </c>
       <c r="G44">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H44">
         <v>31</v>
@@ -44380,7 +44382,7 @@
         <v>39</v>
       </c>
       <c r="G45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H45">
         <v>32</v>
@@ -44400,7 +44402,7 @@
         <v>333</v>
       </c>
       <c r="G46">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H46">
         <v>33</v>
@@ -44420,7 +44422,7 @@
         <v>333</v>
       </c>
       <c r="G47">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H47">
         <v>33</v>
@@ -44437,7 +44439,7 @@
         <v>39</v>
       </c>
       <c r="G48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H48">
         <v>34</v>
@@ -44457,7 +44459,7 @@
         <v>332</v>
       </c>
       <c r="G49">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H49">
         <v>35</v>
@@ -44477,7 +44479,7 @@
         <v>331</v>
       </c>
       <c r="G50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H50">
         <v>36</v>
@@ -44497,7 +44499,7 @@
         <v>330</v>
       </c>
       <c r="G51">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H51">
         <v>37</v>
@@ -44517,7 +44519,7 @@
         <v>329</v>
       </c>
       <c r="G52">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H52">
         <v>38</v>
@@ -44537,7 +44539,7 @@
         <v>328</v>
       </c>
       <c r="G53">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H53">
         <v>39</v>
@@ -44557,7 +44559,7 @@
         <v>327</v>
       </c>
       <c r="G54">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H54">
         <v>40</v>
@@ -44577,7 +44579,7 @@
         <v>326</v>
       </c>
       <c r="G55">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H55">
         <v>41</v>
@@ -44597,7 +44599,7 @@
         <v>325</v>
       </c>
       <c r="G56">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H56">
         <v>42</v>
@@ -44617,7 +44619,7 @@
         <v>324</v>
       </c>
       <c r="G57">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H57">
         <v>44</v>
@@ -44631,7 +44633,7 @@
         <v>39</v>
       </c>
       <c r="G58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H58">
         <v>45</v>
@@ -44648,7 +44650,7 @@
         <v>39</v>
       </c>
       <c r="G59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H59">
         <v>46</v>
@@ -44668,7 +44670,7 @@
         <v>323</v>
       </c>
       <c r="G60">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H60">
         <v>47</v>
@@ -44685,7 +44687,7 @@
         <v>39</v>
       </c>
       <c r="G61">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H61">
         <v>48</v>
@@ -44705,7 +44707,7 @@
         <v>322</v>
       </c>
       <c r="G62">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H62">
         <v>49</v>
@@ -44722,7 +44724,7 @@
         <v>39</v>
       </c>
       <c r="G63">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H63">
         <v>50</v>
@@ -44742,7 +44744,7 @@
         <v>273</v>
       </c>
       <c r="G64">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H64">
         <v>51</v>
@@ -44762,7 +44764,7 @@
         <v>321</v>
       </c>
       <c r="G65">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H65">
         <v>52</v>
@@ -44782,7 +44784,7 @@
         <v>320</v>
       </c>
       <c r="G66">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H66">
         <v>53</v>
@@ -44802,7 +44804,7 @@
         <v>319</v>
       </c>
       <c r="G67">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H67">
         <v>54</v>
@@ -44822,7 +44824,7 @@
         <v>318</v>
       </c>
       <c r="G68">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H68">
         <v>55</v>
@@ -44842,7 +44844,7 @@
         <v>317</v>
       </c>
       <c r="G69">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H69">
         <v>56</v>
@@ -44862,7 +44864,7 @@
         <v>273</v>
       </c>
       <c r="G70">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H70">
         <v>57</v>
@@ -44882,7 +44884,7 @@
         <v>288</v>
       </c>
       <c r="G71">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H71">
         <v>58</v>
@@ -44902,7 +44904,7 @@
         <v>316</v>
       </c>
       <c r="G72">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H72">
         <v>59</v>
@@ -44922,7 +44924,7 @@
         <v>283</v>
       </c>
       <c r="G73">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H73">
         <v>60</v>
@@ -44942,7 +44944,7 @@
         <v>315</v>
       </c>
       <c r="G74">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H74">
         <v>61</v>
@@ -44962,7 +44964,7 @@
         <v>314</v>
       </c>
       <c r="G75">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H75">
         <v>62</v>
@@ -44982,7 +44984,7 @@
         <v>313</v>
       </c>
       <c r="G76">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H76">
         <v>63</v>
@@ -45002,7 +45004,7 @@
         <v>312</v>
       </c>
       <c r="G77">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H77">
         <v>64</v>
@@ -45022,7 +45024,7 @@
         <v>311</v>
       </c>
       <c r="G78">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H78">
         <v>65</v>
@@ -45042,7 +45044,7 @@
         <v>310</v>
       </c>
       <c r="G79">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H79">
         <v>66</v>
@@ -45062,7 +45064,7 @@
         <v>309</v>
       </c>
       <c r="G80">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H80">
         <v>67</v>
@@ -45082,7 +45084,7 @@
         <v>308</v>
       </c>
       <c r="G81">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H81">
         <v>68</v>
@@ -45102,7 +45104,7 @@
         <v>307</v>
       </c>
       <c r="G82">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H82">
         <v>69</v>
@@ -45122,7 +45124,7 @@
         <v>306</v>
       </c>
       <c r="G83">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H83">
         <v>70</v>
@@ -45142,7 +45144,7 @@
         <v>305</v>
       </c>
       <c r="G84">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H84">
         <v>71</v>
@@ -45156,7 +45158,7 @@
         <v>46</v>
       </c>
       <c r="G85">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H85">
         <v>72</v>
@@ -45176,7 +45178,7 @@
         <v>279</v>
       </c>
       <c r="G86">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H86">
         <v>73</v>
@@ -45193,7 +45195,7 @@
         <v>39</v>
       </c>
       <c r="G87">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H87">
         <v>74</v>
@@ -45210,7 +45212,7 @@
         <v>46</v>
       </c>
       <c r="G88">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H88">
         <v>75</v>
@@ -45218,25 +45220,25 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H22:H26">
-    <cfRule type="duplicateValues" dxfId="9" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H30:H35">
-    <cfRule type="duplicateValues" dxfId="8" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H37:H39">
-    <cfRule type="duplicateValues" dxfId="7" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H45:H48">
-    <cfRule type="duplicateValues" dxfId="6" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H51:H54">
-    <cfRule type="duplicateValues" dxfId="5" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H56:H64">
-    <cfRule type="duplicateValues" dxfId="4" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H67:H88">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>